<commit_message>
termine la fucnion de los botnes cargar masivo y ajustes de los botones de cada universdad
</commit_message>
<xml_diff>
--- a/ofertas_de_empleo.xlsx
+++ b/ofertas_de_empleo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\universidades\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Universidaterminada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD4C2D9-4B3D-4192-BF1D-7C54C5D15753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83753765-A562-4CB1-82FF-0DAAEA049D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="72">
   <si>
     <t>título de la oferta</t>
   </si>
@@ -82,10 +82,16 @@
     <t>tiempo dedicado</t>
   </si>
   <si>
+    <t>universidades</t>
+  </si>
+  <si>
+    <t>medico</t>
+  </si>
+  <si>
     <t>salud</t>
   </si>
   <si>
-    <t>medico</t>
+    <t xml:space="preserve">adminitrador </t>
   </si>
   <si>
     <t>Profesional</t>
@@ -124,6 +130,9 @@
     <t>Mensual</t>
   </si>
   <si>
+    <t>Areandina</t>
+  </si>
+  <si>
     <t>cordinador trade</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
     <t>la vega</t>
   </si>
   <si>
+    <t>militar</t>
+  </si>
+  <si>
     <t xml:space="preserve">kam </t>
   </si>
   <si>
@@ -154,6 +166,9 @@
     <t>bogota</t>
   </si>
   <si>
+    <t>Simonbolivar</t>
+  </si>
+  <si>
     <t>ejecutivo comercial</t>
   </si>
   <si>
@@ -221,9 +236,6 @@
   </si>
   <si>
     <t>$4 a $14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adminitrador </t>
   </si>
 </sst>
 </file>
@@ -586,24 +598,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,52 +667,55 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -721,57 +727,60 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T2" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P3">
         <v>2</v>
@@ -783,57 +792,60 @@
         <v>2</v>
       </c>
       <c r="S3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T3" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="U3" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P4">
         <v>3</v>
@@ -845,57 +857,60 @@
         <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T4" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P5">
         <v>4</v>
@@ -907,57 +922,57 @@
         <v>4</v>
       </c>
       <c r="S5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P6">
         <v>5</v>
@@ -969,57 +984,57 @@
         <v>5</v>
       </c>
       <c r="S6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P7">
         <v>6</v>
@@ -1031,57 +1046,57 @@
         <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P8">
         <v>7</v>
@@ -1093,57 +1108,57 @@
         <v>7</v>
       </c>
       <c r="S8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="K9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P9">
         <v>8</v>
@@ -1155,57 +1170,57 @@
         <v>8</v>
       </c>
       <c r="S9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
         <v>51</v>
       </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P10">
         <v>9</v>
@@ -1217,57 +1232,57 @@
         <v>9</v>
       </c>
       <c r="S10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P11">
         <v>10</v>
@@ -1279,57 +1294,57 @@
         <v>10</v>
       </c>
       <c r="S11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P12">
         <v>11</v>
@@ -1341,10 +1356,10 @@
         <v>11</v>
       </c>
       <c r="S12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>